<commit_message>
add user case chinh sua profile
</commit_message>
<xml_diff>
--- a/Telegram02_Software Requirement Specification.xlsx
+++ b/Telegram02_Software Requirement Specification.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ha\Desktop\Final CNPM\Software-Engineering-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4548D9-39A4-4E26-8055-F52481E4C72E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228E5CE0-456A-4A20-8605-EB4A9CB1A73B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="705" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="705" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Record of change" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,9 @@
     <sheet name="3.1.9 UC_CS thông báo tin nhắn" sheetId="33" r:id="rId13"/>
     <sheet name="3.1.10 UC_CS thông báo nhóm" sheetId="34" r:id="rId14"/>
     <sheet name="3.1.11 UC_Quyền riêngtư,bảo mật" sheetId="35" r:id="rId15"/>
-    <sheet name="3.1.12 UC_CapNhatThongTinCaNhan" sheetId="36" r:id="rId16"/>
-    <sheet name="3.1.13 UC_CapNhatAvatar" sheetId="37" r:id="rId17"/>
+    <sheet name="3.1.12 UC_CS cai dat chat" sheetId="36" r:id="rId16"/>
+    <sheet name="3.1.13 UC_Chinh sua profile" sheetId="37" r:id="rId17"/>
+    <sheet name="Sheet1" sheetId="38" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'1.Introduction'!$A$1:$AJ$55</definedName>
@@ -38,8 +39,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">'3.1.1 UC_Đăng nhập'!$A$1:$AJ$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">'3.1.10 UC_CS thông báo nhóm'!$A$1:$AJ$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="14">'3.1.11 UC_Quyền riêngtư,bảo mật'!$A$1:$AJ$56</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="15">'3.1.12 UC_CapNhatThongTinCaNhan'!$A$1:$AJ$59</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="16">'3.1.13 UC_CapNhatAvatar'!$A$1:$AJ$59</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="15">'3.1.12 UC_CS cai dat chat'!$A$1:$AJ$59</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="16">'3.1.13 UC_Chinh sua profile'!$A$1:$AJ$59</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'3.1.2 UC_Nhập số điện thoại'!$A$1:$AJ$67</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'3.1.3 UC_Chat với một người'!$A$1:$AJ$60</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'3.1.4 UC_Gửi tin nhắn'!$A$1:$AJ$60</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="223">
   <si>
     <t>Date</t>
   </si>
@@ -373,34 +374,10 @@
     <t>External</t>
   </si>
   <si>
-    <t>Nhân viên đã đăng nhập vào hệ thống.</t>
-  </si>
-  <si>
     <t>ID: SI UC 003</t>
   </si>
   <si>
-    <t>NhanVien, NhanVienNhanSu</t>
-  </si>
-  <si>
     <t>chọn.</t>
-  </si>
-  <si>
-    <t>3. Nhân viên nhập thông tin cần chỉnh sửa.</t>
-  </si>
-  <si>
-    <t>4. Hệ thống kiểm tra dữ liệu nhập trên form.</t>
-  </si>
-  <si>
-    <t>5. Nhân viên ấn nút "Save" để lưu thông tin.</t>
-  </si>
-  <si>
-    <t>6. Hệ thống hiện popup yêu cầu xác nhận.</t>
-  </si>
-  <si>
-    <t>8. Hệ thống update dữ liệu và hiện thông báo cập nhật thành công.</t>
-  </si>
-  <si>
-    <t>4.1. Nếu dữ liệu không hợp lệ, nút "Save" sẽ disenble.</t>
   </si>
   <si>
     <t>Dữ liệu cập nhật hợp lệ.</t>
@@ -421,27 +398,6 @@
     <t>ID: SI UC 004</t>
   </si>
   <si>
-    <t>Chức năng này cho phép nhân viên cập nhật thông tin cá nhân của bản thân. Nếu là quyền nhân viên quản lý nhân sự thì có thể cập nhật thông tin cá nhân của bản thân và các nhân viên khác.</t>
-  </si>
-  <si>
-    <t>1. Nhân viên ấn vào nút "Edit Information"</t>
-  </si>
-  <si>
-    <t>2. Hệ thống hiển thị form chỉnh sửa thông tin cá nhân của nhân viên</t>
-  </si>
-  <si>
-    <t>7. Nhân viên chọn "OK".</t>
-  </si>
-  <si>
-    <t>7.1. Nhân viên chọn "Cancel" sẽ hủy thao tác cập nhật.</t>
-  </si>
-  <si>
-    <t>Cập nhật thành công thông tin cá nhân.</t>
-  </si>
-  <si>
-    <t>Cho phép cập  thông tin cá nhân.</t>
-  </si>
-  <si>
     <t>ID: SI UC 009</t>
   </si>
   <si>
@@ -452,36 +408,6 @@
   </si>
   <si>
     <t>ID: SI UC 012</t>
-  </si>
-  <si>
-    <t>Cap nhat avatar</t>
-  </si>
-  <si>
-    <t>Chức năng này cho phép nhân viên cập nhật ảnh đại diện cá nhân của bản thân. Nếu là quyền nhân viên quản lý nhân sự thì có thể cập ảnh đại diện cá nhân của bản thân và các nhân viên khác.</t>
-  </si>
-  <si>
-    <t>1. Nhân viên ấn vào nút "Change avatar"</t>
-  </si>
-  <si>
-    <t>3. Nhân viên nhập URL ảnh.</t>
-  </si>
-  <si>
-    <t>2. Hệ thống hiển thị form nhập URL ảnh(URL online).</t>
-  </si>
-  <si>
-    <t>5. Nhân viên ấn nút "Preview" để xem ảnh.</t>
-  </si>
-  <si>
-    <t>6. Hệ thống xử lý và hiển thị ảnh từ URL được nhập.</t>
-  </si>
-  <si>
-    <t>4.1. Nếu dữ liệu không hợp lệ, sẽ thông báo "Invalid URL"</t>
-  </si>
-  <si>
-    <t>Cập nhật thành công avatar cá nhân.</t>
-  </si>
-  <si>
-    <t>Cho phép cập nhật avatar cá nhân.</t>
   </si>
   <si>
     <t>ID: SI UC 013</t>
@@ -805,7 +731,37 @@
     <t>Cho phép xem các cài đặt hiện tại.</t>
   </si>
   <si>
-    <t>Chỉnh sửa quyền riêng tư và bảo mật</t>
+    <t>Chỉnh sửa cài đặt chat</t>
+  </si>
+  <si>
+    <t>Chức năng này cho phép người dùng chỉnh sửa cài đặt trong khi chat, tự động tải về ảnh, audio hoặc không.</t>
+  </si>
+  <si>
+    <t>1. Người dùng Switch tắt chức năng</t>
+  </si>
+  <si>
+    <t>2. Hệ thống lưu lại thay đổi người dùng.</t>
+  </si>
+  <si>
+    <t>Cập nhật các thay đổi của người dùng ngay lâp tức</t>
+  </si>
+  <si>
+    <t>Cho phép người dùng switch on off</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa profile</t>
+  </si>
+  <si>
+    <t>Chức năng này cho phép người dùng chỉnh sửa các thông tin profile của người dùng và chỉnh sửa chat background</t>
+  </si>
+  <si>
+    <t>1.Người dùng ấn vào mục "Cài đặt"</t>
+  </si>
+  <si>
+    <t>2. Hệ thống hiện thị các thông tin profile hiện tại.</t>
+  </si>
+  <si>
+    <t>Cho phép cập nhật profile cá nhân</t>
   </si>
 </sst>
 </file>
@@ -2814,7 +2770,7 @@
           <xdr:col>30</xdr:col>
           <xdr:colOff>219075</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>152399</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2824,7 +2780,127 @@
                   <a14:compatExt spid="_x0000_s25602"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C12AEF2F-0CD7-4B56-8CD7-BA77FF892E9C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002640000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>35</xdr:col>
+          <xdr:colOff>247650</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="27651" name="Object 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s27651"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-0000036C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>171450</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>29</xdr:col>
+          <xdr:colOff>114300</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="28673" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s28673"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B20963A2-A6AB-4EBA-B49F-03143E744A8C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2869,55 +2945,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>94447</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>28170</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1381125" y="1733550"/>
-          <a:ext cx="6428572" cy="3238095"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3749,6 +3776,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -3954,6 +3982,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -3970,7 +3999,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -5034,7 +5063,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -5061,7 +5090,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -5076,7 +5105,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -5116,7 +5145,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -5156,7 +5185,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -5232,7 +5261,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
       <c r="F37" s="189" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="G37" s="189"/>
       <c r="H37" s="189"/>
@@ -5420,7 +5449,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -5439,7 +5468,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="97" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -5460,7 +5489,7 @@
     </row>
     <row r="43" spans="2:35">
       <c r="B43" s="94" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="C43" s="95"/>
       <c r="D43" s="95"/>
@@ -5479,7 +5508,7 @@
       <c r="Q43" s="95"/>
       <c r="R43" s="96"/>
       <c r="S43" s="94" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="T43" s="95"/>
       <c r="U43" s="95"/>
@@ -5500,7 +5529,7 @@
     </row>
     <row r="44" spans="2:35">
       <c r="B44" s="94" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="C44" s="95"/>
       <c r="D44" s="95"/>
@@ -5519,7 +5548,7 @@
       <c r="Q44" s="95"/>
       <c r="R44" s="96"/>
       <c r="S44" s="94" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="T44" s="95"/>
       <c r="U44" s="95"/>
@@ -5690,7 +5719,7 @@
     </row>
     <row r="49" spans="2:35">
       <c r="B49" s="97" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="C49" s="92"/>
       <c r="D49" s="92"/>
@@ -5709,7 +5738,7 @@
       <c r="Q49" s="92"/>
       <c r="R49" s="93"/>
       <c r="S49" s="97" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="T49" s="92"/>
       <c r="U49" s="92"/>
@@ -5730,7 +5759,7 @@
     </row>
     <row r="50" spans="2:35">
       <c r="B50" s="94" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="C50" s="95"/>
       <c r="D50" s="95"/>
@@ -5810,7 +5839,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
       <c r="F52" s="189" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="G52" s="189"/>
       <c r="H52" s="189"/>
@@ -5850,7 +5879,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
       <c r="F53" s="189" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
@@ -5890,7 +5919,7 @@
       <c r="D54" s="51"/>
       <c r="E54" s="51"/>
       <c r="F54" s="189" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
       <c r="G54" s="189"/>
       <c r="H54" s="189"/>
@@ -5930,7 +5959,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="189" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G55" s="189"/>
       <c r="H55" s="189"/>
@@ -6157,6 +6186,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -6173,7 +6203,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -7237,7 +7267,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -7264,7 +7294,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -7279,7 +7309,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -7319,7 +7349,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -7359,7 +7389,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -7621,7 +7651,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -7640,7 +7670,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="94" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -7998,7 +8028,7 @@
       <c r="E52" s="51"/>
       <c r="F52" s="51"/>
       <c r="G52" s="133" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="H52" s="131"/>
       <c r="I52" s="131"/>
@@ -8333,6 +8363,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -8349,7 +8380,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -9413,7 +9444,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -9440,7 +9471,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -9455,7 +9486,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -9495,7 +9526,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -9535,7 +9566,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -9797,7 +9828,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -9816,7 +9847,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="94" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -10173,7 +10204,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
       <c r="F52" s="189" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="G52" s="189"/>
       <c r="H52" s="189"/>
@@ -10516,6 +10547,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AJ56"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A36" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -10532,7 +10564,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -11596,7 +11628,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -11623,7 +11655,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -11638,7 +11670,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -11678,7 +11710,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -11718,7 +11750,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -11997,7 +12029,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="94" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -12018,7 +12050,7 @@
     </row>
     <row r="43" spans="2:35">
       <c r="B43" s="97" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="C43" s="92"/>
       <c r="D43" s="92"/>
@@ -12073,7 +12105,7 @@
       <c r="Q44" s="95"/>
       <c r="R44" s="96"/>
       <c r="S44" s="94" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="T44" s="95"/>
       <c r="U44" s="95"/>
@@ -12286,7 +12318,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="51"/>
       <c r="F50" s="189" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="G50" s="189"/>
       <c r="H50" s="189"/>
@@ -12326,7 +12358,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="51"/>
       <c r="F51" s="189" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="G51" s="189"/>
       <c r="H51" s="189"/>
@@ -12406,7 +12438,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
       <c r="F53" s="189" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
@@ -12633,6 +12665,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AJ56"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -13713,7 +13746,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -13740,7 +13773,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -13755,7 +13788,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -13795,7 +13828,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -13835,7 +13868,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -14114,7 +14147,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="94" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -14135,7 +14168,7 @@
     </row>
     <row r="43" spans="2:35">
       <c r="B43" s="97" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="C43" s="92"/>
       <c r="D43" s="92"/>
@@ -14190,7 +14223,7 @@
       <c r="Q44" s="95"/>
       <c r="R44" s="96"/>
       <c r="S44" s="94" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="T44" s="95"/>
       <c r="U44" s="95"/>
@@ -14403,7 +14436,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="51"/>
       <c r="F50" s="189" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="G50" s="189"/>
       <c r="H50" s="189"/>
@@ -14443,7 +14476,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="51"/>
       <c r="F51" s="189" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="G51" s="189"/>
       <c r="H51" s="189"/>
@@ -14523,7 +14556,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
       <c r="F53" s="189" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
@@ -14750,9 +14783,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:AJ56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A26" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="AC60" sqref="AC60"/>
     </sheetView>
   </sheetViews>
@@ -15830,7 +15864,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -15857,7 +15891,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -15872,7 +15906,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -15912,7 +15946,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -15952,7 +15986,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -16214,7 +16248,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -16233,7 +16267,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="94" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -16254,7 +16288,7 @@
     </row>
     <row r="43" spans="2:35">
       <c r="B43" s="97" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="C43" s="92"/>
       <c r="D43" s="92"/>
@@ -16273,7 +16307,7 @@
       <c r="Q43" s="92"/>
       <c r="R43" s="93"/>
       <c r="S43" s="94" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="T43" s="92"/>
       <c r="U43" s="92"/>
@@ -16294,7 +16328,7 @@
     </row>
     <row r="44" spans="2:35">
       <c r="B44" s="94" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="C44" s="95"/>
       <c r="D44" s="95"/>
@@ -16410,7 +16444,7 @@
     </row>
     <row r="47" spans="2:35">
       <c r="B47" s="97" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="C47" s="92"/>
       <c r="D47" s="92"/>
@@ -16526,7 +16560,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="51"/>
       <c r="F50" s="189" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="G50" s="189"/>
       <c r="H50" s="189"/>
@@ -16646,7 +16680,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
       <c r="F53" s="189" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
@@ -16872,11 +16906,12 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
@@ -16889,7 +16924,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -17953,7 +17988,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -17980,7 +18015,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -17995,7 +18030,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -18035,7 +18070,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -18075,7 +18110,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>109</v>
+        <v>213</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -18337,7 +18372,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>110</v>
+        <v>214</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -18356,7 +18391,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="97" t="s">
-        <v>111</v>
+        <v>215</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -18376,9 +18411,7 @@
       <c r="AI42" s="93"/>
     </row>
     <row r="43" spans="2:35">
-      <c r="B43" s="94" t="s">
-        <v>97</v>
-      </c>
+      <c r="B43" s="94"/>
       <c r="C43" s="95"/>
       <c r="D43" s="95"/>
       <c r="E43" s="95"/>
@@ -18395,9 +18428,7 @@
       <c r="P43" s="95"/>
       <c r="Q43" s="95"/>
       <c r="R43" s="96"/>
-      <c r="S43" s="94" t="s">
-        <v>98</v>
-      </c>
+      <c r="S43" s="94"/>
       <c r="T43" s="95"/>
       <c r="U43" s="95"/>
       <c r="V43" s="95"/>
@@ -18416,9 +18447,7 @@
       <c r="AI43" s="96"/>
     </row>
     <row r="44" spans="2:35">
-      <c r="B44" s="94" t="s">
-        <v>99</v>
-      </c>
+      <c r="B44" s="94"/>
       <c r="C44" s="95"/>
       <c r="D44" s="95"/>
       <c r="E44" s="95"/>
@@ -18435,9 +18464,7 @@
       <c r="P44" s="95"/>
       <c r="Q44" s="95"/>
       <c r="R44" s="96"/>
-      <c r="S44" s="94" t="s">
-        <v>100</v>
-      </c>
+      <c r="S44" s="94"/>
       <c r="T44" s="95"/>
       <c r="U44" s="95"/>
       <c r="V44" s="95"/>
@@ -18456,9 +18483,7 @@
       <c r="AI44" s="96"/>
     </row>
     <row r="45" spans="2:35">
-      <c r="B45" s="94" t="s">
-        <v>112</v>
-      </c>
+      <c r="B45" s="94"/>
       <c r="C45" s="95"/>
       <c r="D45" s="95"/>
       <c r="E45" s="95"/>
@@ -18475,9 +18500,7 @@
       <c r="P45" s="95"/>
       <c r="Q45" s="95"/>
       <c r="R45" s="96"/>
-      <c r="S45" s="94" t="s">
-        <v>101</v>
-      </c>
+      <c r="S45" s="94"/>
       <c r="T45" s="95"/>
       <c r="U45" s="95"/>
       <c r="V45" s="95"/>
@@ -18610,9 +18633,7 @@
       <c r="AI48" s="70"/>
     </row>
     <row r="49" spans="2:35">
-      <c r="B49" s="97" t="s">
-        <v>113</v>
-      </c>
+      <c r="B49" s="97"/>
       <c r="C49" s="92"/>
       <c r="D49" s="92"/>
       <c r="E49" s="92"/>
@@ -18629,9 +18650,7 @@
       <c r="P49" s="92"/>
       <c r="Q49" s="92"/>
       <c r="R49" s="93"/>
-      <c r="S49" s="97" t="s">
-        <v>102</v>
-      </c>
+      <c r="S49" s="97"/>
       <c r="T49" s="92"/>
       <c r="U49" s="92"/>
       <c r="V49" s="92"/>
@@ -18729,7 +18748,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
       <c r="F52" s="189" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="G52" s="189"/>
       <c r="H52" s="189"/>
@@ -18769,7 +18788,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
       <c r="F53" s="189" t="s">
-        <v>114</v>
+        <v>216</v>
       </c>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
@@ -18808,9 +18827,7 @@
       <c r="C54" s="51"/>
       <c r="D54" s="51"/>
       <c r="E54" s="51"/>
-      <c r="F54" s="189" t="s">
-        <v>103</v>
-      </c>
+      <c r="F54" s="189"/>
       <c r="G54" s="189"/>
       <c r="H54" s="189"/>
       <c r="I54" s="189"/>
@@ -18849,7 +18866,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="189" t="s">
-        <v>115</v>
+        <v>217</v>
       </c>
       <c r="G55" s="189"/>
       <c r="H55" s="189"/>
@@ -19042,15 +19059,45 @@
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Visio.Drawing.15" shapeId="27651" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>35</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>22</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Visio.Drawing.15" shapeId="27651" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15"/>
@@ -19063,7 +19110,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -20127,7 +20174,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>120</v>
+        <v>218</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -20154,7 +20201,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -20169,7 +20216,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -20209,7 +20256,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -20249,7 +20296,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>121</v>
+        <v>219</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -20511,7 +20558,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>122</v>
+        <v>220</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -20530,7 +20577,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="97" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -20550,9 +20597,7 @@
       <c r="AI42" s="93"/>
     </row>
     <row r="43" spans="2:35">
-      <c r="B43" s="94" t="s">
-        <v>123</v>
-      </c>
+      <c r="B43" s="94"/>
       <c r="C43" s="95"/>
       <c r="D43" s="95"/>
       <c r="E43" s="95"/>
@@ -20569,9 +20614,7 @@
       <c r="P43" s="95"/>
       <c r="Q43" s="95"/>
       <c r="R43" s="96"/>
-      <c r="S43" s="94" t="s">
-        <v>98</v>
-      </c>
+      <c r="S43" s="94"/>
       <c r="T43" s="95"/>
       <c r="U43" s="95"/>
       <c r="V43" s="95"/>
@@ -20590,9 +20633,7 @@
       <c r="AI43" s="96"/>
     </row>
     <row r="44" spans="2:35">
-      <c r="B44" s="94" t="s">
-        <v>125</v>
-      </c>
+      <c r="B44" s="94"/>
       <c r="C44" s="95"/>
       <c r="D44" s="95"/>
       <c r="E44" s="95"/>
@@ -20609,9 +20650,7 @@
       <c r="P44" s="95"/>
       <c r="Q44" s="95"/>
       <c r="R44" s="96"/>
-      <c r="S44" s="94" t="s">
-        <v>126</v>
-      </c>
+      <c r="S44" s="94"/>
       <c r="T44" s="95"/>
       <c r="U44" s="95"/>
       <c r="V44" s="95"/>
@@ -20630,9 +20669,7 @@
       <c r="AI44" s="96"/>
     </row>
     <row r="45" spans="2:35">
-      <c r="B45" s="94" t="s">
-        <v>112</v>
-      </c>
+      <c r="B45" s="94"/>
       <c r="C45" s="95"/>
       <c r="D45" s="95"/>
       <c r="E45" s="95"/>
@@ -20649,9 +20686,7 @@
       <c r="P45" s="95"/>
       <c r="Q45" s="95"/>
       <c r="R45" s="96"/>
-      <c r="S45" s="94" t="s">
-        <v>101</v>
-      </c>
+      <c r="S45" s="94"/>
       <c r="T45" s="95"/>
       <c r="U45" s="95"/>
       <c r="V45" s="95"/>
@@ -20784,9 +20819,7 @@
       <c r="AI48" s="70"/>
     </row>
     <row r="49" spans="2:35">
-      <c r="B49" s="97" t="s">
-        <v>113</v>
-      </c>
+      <c r="B49" s="97"/>
       <c r="C49" s="92"/>
       <c r="D49" s="92"/>
       <c r="E49" s="92"/>
@@ -20803,9 +20836,7 @@
       <c r="P49" s="92"/>
       <c r="Q49" s="92"/>
       <c r="R49" s="93"/>
-      <c r="S49" s="97" t="s">
-        <v>127</v>
-      </c>
+      <c r="S49" s="97"/>
       <c r="T49" s="92"/>
       <c r="U49" s="92"/>
       <c r="V49" s="92"/>
@@ -20903,7 +20934,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
       <c r="F52" s="189" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="G52" s="189"/>
       <c r="H52" s="189"/>
@@ -20942,9 +20973,7 @@
       <c r="C53" s="51"/>
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
-      <c r="F53" s="189" t="s">
-        <v>128</v>
-      </c>
+      <c r="F53" s="189"/>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
       <c r="I53" s="189"/>
@@ -20982,9 +21011,7 @@
       <c r="C54" s="51"/>
       <c r="D54" s="51"/>
       <c r="E54" s="51"/>
-      <c r="F54" s="189" t="s">
-        <v>103</v>
-      </c>
+      <c r="F54" s="189"/>
       <c r="G54" s="189"/>
       <c r="H54" s="189"/>
       <c r="I54" s="189"/>
@@ -21023,7 +21050,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="189" t="s">
-        <v>129</v>
+        <v>222</v>
       </c>
       <c r="G55" s="189"/>
       <c r="H55" s="189"/>
@@ -21217,11 +21244,55 @@
     <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Visio.Drawing.15" shapeId="28673" r:id="rId4">
+          <objectPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>29</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Visio.Drawing.15" shapeId="28673" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C40026F-7338-4957-BD21-4AF8AA8EE850}">
+  <sheetPr codeName="Sheet18"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AJ52"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A24" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -23089,6 +23160,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AJ37"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -23105,7 +23177,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -24582,9 +24654,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AJ31"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="BF14" sqref="BF14"/>
     </sheetView>
   </sheetViews>
@@ -24598,7 +24671,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -25860,6 +25933,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AJ55"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -25876,7 +25950,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -26789,7 +26863,7 @@
       <c r="D27" s="57"/>
       <c r="E27" s="57"/>
       <c r="F27" s="176" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="G27" s="177"/>
       <c r="H27" s="177"/>
@@ -26816,7 +26890,7 @@
       <c r="AC27" s="177"/>
       <c r="AD27" s="178"/>
       <c r="AE27" s="136" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="AF27" s="134"/>
       <c r="AG27" s="134"/>
@@ -26831,7 +26905,7 @@
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
       <c r="F28" s="179" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G28" s="180"/>
       <c r="H28" s="180"/>
@@ -26871,7 +26945,7 @@
       <c r="D29" s="61"/>
       <c r="E29" s="61"/>
       <c r="F29" s="182" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G29" s="160"/>
       <c r="H29" s="160"/>
@@ -26911,7 +26985,7 @@
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
       <c r="F30" s="185" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="G30" s="158"/>
       <c r="H30" s="158"/>
@@ -26987,7 +27061,7 @@
       <c r="D32" s="51"/>
       <c r="E32" s="51"/>
       <c r="F32" s="185" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="G32" s="158"/>
       <c r="H32" s="158"/>
@@ -27175,7 +27249,7 @@
     </row>
     <row r="37" spans="2:35">
       <c r="B37" s="145" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="C37" s="146"/>
       <c r="D37" s="147"/>
@@ -27194,7 +27268,7 @@
       <c r="Q37" s="146"/>
       <c r="R37" s="148"/>
       <c r="S37" s="149" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="T37" s="92"/>
       <c r="U37" s="92"/>
@@ -27382,7 +27456,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="150" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -27705,7 +27779,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="51"/>
       <c r="F51" s="184" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="G51" s="160"/>
       <c r="H51" s="160"/>
@@ -27745,7 +27819,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
       <c r="F52" s="184" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="G52" s="160"/>
       <c r="H52" s="160"/>
@@ -27971,6 +28045,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AJ66"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -27987,7 +28062,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -29051,7 +29126,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="188" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="G32" s="173"/>
       <c r="H32" s="173"/>
@@ -29078,7 +29153,7 @@
       <c r="AC32" s="173"/>
       <c r="AD32" s="174"/>
       <c r="AE32" s="89" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="AF32" s="90"/>
       <c r="AG32" s="90"/>
@@ -29093,7 +29168,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -29133,7 +29208,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -29173,7 +29248,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -29249,7 +29324,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
       <c r="F37" s="185" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="G37" s="158"/>
       <c r="H37" s="158"/>
@@ -29437,7 +29512,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="140" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="C42" s="143"/>
       <c r="D42" s="142"/>
@@ -29456,7 +29531,7 @@
       <c r="Q42" s="138"/>
       <c r="R42" s="139"/>
       <c r="S42" s="144" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="T42" s="138"/>
       <c r="U42" s="92"/>
@@ -29494,7 +29569,7 @@
       <c r="Q43" s="95"/>
       <c r="R43" s="96"/>
       <c r="S43" s="97" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="T43" s="95"/>
       <c r="U43" s="95"/>
@@ -29515,7 +29590,7 @@
     </row>
     <row r="44" spans="2:35">
       <c r="B44" s="94" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C44" s="95"/>
       <c r="D44" s="95"/>
@@ -29570,7 +29645,7 @@
       <c r="Q45" s="95"/>
       <c r="R45" s="96"/>
       <c r="S45" s="94" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="T45" s="95"/>
       <c r="U45" s="95"/>
@@ -29608,7 +29683,7 @@
       <c r="Q46" s="95"/>
       <c r="R46" s="96"/>
       <c r="S46" s="94" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="T46" s="95"/>
       <c r="U46" s="95"/>
@@ -29868,7 +29943,7 @@
       <c r="Q53" s="92"/>
       <c r="R53" s="93"/>
       <c r="S53" s="97" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="T53" s="92"/>
       <c r="U53" s="92"/>
@@ -29906,7 +29981,7 @@
       <c r="Q54" s="95"/>
       <c r="R54" s="96"/>
       <c r="S54" s="94" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="T54" s="95"/>
       <c r="U54" s="95"/>
@@ -30113,7 +30188,7 @@
       <c r="D60" s="51"/>
       <c r="E60" s="51"/>
       <c r="F60" s="184" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="G60" s="160"/>
       <c r="H60" s="160"/>
@@ -30233,7 +30308,7 @@
       <c r="D63" s="51"/>
       <c r="E63" s="51"/>
       <c r="F63" s="184" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="G63" s="160"/>
       <c r="H63" s="160"/>
@@ -30459,6 +30534,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AJ59"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -30475,7 +30551,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -31539,7 +31615,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -31566,7 +31642,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -31581,7 +31657,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -31621,7 +31697,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -31661,7 +31737,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -31737,7 +31813,7 @@
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
       <c r="F37" s="189" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="G37" s="189"/>
       <c r="H37" s="189"/>
@@ -31925,7 +32001,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -31943,7 +32019,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="97" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -31981,7 +32057,7 @@
       <c r="Q43" s="95"/>
       <c r="R43" s="96"/>
       <c r="S43" s="94" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T43" s="95"/>
       <c r="U43" s="95"/>
@@ -32002,7 +32078,7 @@
     </row>
     <row r="44" spans="2:35">
       <c r="B44" s="94" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C44" s="95"/>
       <c r="D44" s="95"/>
@@ -32021,7 +32097,7 @@
       <c r="Q44" s="95"/>
       <c r="R44" s="96"/>
       <c r="S44" s="94" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="T44" s="95"/>
       <c r="U44" s="95"/>
@@ -32245,7 +32321,7 @@
       <c r="Q50" s="92"/>
       <c r="R50" s="93"/>
       <c r="S50" s="97" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="T50" s="92"/>
       <c r="U50" s="92"/>
@@ -32283,7 +32359,7 @@
       <c r="Q51" s="95"/>
       <c r="R51" s="96"/>
       <c r="S51" s="94" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="T51" s="95"/>
       <c r="U51" s="95"/>
@@ -32346,7 +32422,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
       <c r="F53" s="189" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
@@ -32426,7 +32502,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="189" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G55" s="189"/>
       <c r="H55" s="189"/>
@@ -32466,7 +32542,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="51"/>
       <c r="F56" s="189" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="G56" s="189"/>
       <c r="H56" s="189"/>
@@ -32693,6 +32769,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AJ61"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -32709,7 +32786,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -33773,7 +33850,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -33800,7 +33877,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -33815,7 +33892,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -33855,7 +33932,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -33895,7 +33972,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -34157,7 +34234,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -34176,7 +34253,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="97" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -34197,7 +34274,7 @@
     </row>
     <row r="43" spans="2:35">
       <c r="B43" s="94" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="C43" s="95"/>
       <c r="D43" s="95"/>
@@ -34216,7 +34293,7 @@
       <c r="Q43" s="95"/>
       <c r="R43" s="96"/>
       <c r="S43" s="94" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="T43" s="95"/>
       <c r="U43" s="95"/>
@@ -34273,7 +34350,7 @@
     </row>
     <row r="45" spans="2:35">
       <c r="B45" s="94" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="C45" s="95"/>
       <c r="D45" s="95"/>
@@ -34292,7 +34369,7 @@
       <c r="Q45" s="95"/>
       <c r="R45" s="96"/>
       <c r="S45" s="94" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="T45" s="95"/>
       <c r="U45" s="95"/>
@@ -34313,7 +34390,7 @@
     </row>
     <row r="46" spans="2:35">
       <c r="B46" s="94" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="C46" s="95"/>
       <c r="D46" s="95"/>
@@ -34332,7 +34409,7 @@
       <c r="Q46" s="95"/>
       <c r="R46" s="96"/>
       <c r="S46" s="94" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="T46" s="95"/>
       <c r="U46" s="95"/>
@@ -34353,7 +34430,7 @@
     </row>
     <row r="47" spans="2:35">
       <c r="B47" s="94" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="C47" s="95"/>
       <c r="D47" s="95"/>
@@ -34372,7 +34449,7 @@
       <c r="Q47" s="95"/>
       <c r="R47" s="96"/>
       <c r="S47" s="94" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="T47" s="95"/>
       <c r="U47" s="95"/>
@@ -34393,7 +34470,7 @@
     </row>
     <row r="48" spans="2:35">
       <c r="B48" s="94" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="C48" s="95"/>
       <c r="D48" s="95"/>
@@ -34412,7 +34489,7 @@
       <c r="Q48" s="95"/>
       <c r="R48" s="96"/>
       <c r="S48" s="94" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="T48" s="95"/>
       <c r="U48" s="95"/>
@@ -34547,7 +34624,7 @@
     </row>
     <row r="52" spans="2:35">
       <c r="B52" s="97" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="C52" s="92"/>
       <c r="D52" s="92"/>
@@ -34566,7 +34643,7 @@
       <c r="Q52" s="92"/>
       <c r="R52" s="93"/>
       <c r="S52" s="97" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="T52" s="92"/>
       <c r="U52" s="92"/>
@@ -34604,7 +34681,7 @@
       <c r="Q53" s="95"/>
       <c r="R53" s="96"/>
       <c r="S53" s="94" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="T53" s="95"/>
       <c r="U53" s="95"/>
@@ -34667,7 +34744,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="193" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="G55" s="194"/>
       <c r="H55" s="194"/>
@@ -34707,7 +34784,7 @@
       <c r="D56" s="51"/>
       <c r="E56" s="51"/>
       <c r="F56" s="193" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="G56" s="194"/>
       <c r="H56" s="194"/>
@@ -34747,7 +34824,7 @@
       <c r="D57" s="51"/>
       <c r="E57" s="51"/>
       <c r="F57" s="193" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G57" s="194"/>
       <c r="H57" s="194"/>
@@ -34787,7 +34864,7 @@
       <c r="D58" s="51"/>
       <c r="E58" s="51"/>
       <c r="F58" s="193" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="G58" s="194"/>
       <c r="H58" s="194"/>
@@ -35014,6 +35091,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AJ58"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -35030,7 +35108,7 @@
       <c r="C1" s="158"/>
       <c r="D1" s="158"/>
       <c r="E1" s="161" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="F1" s="158"/>
       <c r="G1" s="158"/>
@@ -36094,7 +36172,7 @@
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
       <c r="F32" s="189" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="G32" s="189"/>
       <c r="H32" s="189"/>
@@ -36121,7 +36199,7 @@
       <c r="AC32" s="189"/>
       <c r="AD32" s="189"/>
       <c r="AE32" s="190" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="AF32" s="191"/>
       <c r="AG32" s="191"/>
@@ -36136,7 +36214,7 @@
       <c r="D33" s="51"/>
       <c r="E33" s="51"/>
       <c r="F33" s="188" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="G33" s="173"/>
       <c r="H33" s="173"/>
@@ -36176,7 +36254,7 @@
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="188" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="G34" s="173"/>
       <c r="H34" s="173"/>
@@ -36216,7 +36294,7 @@
       <c r="D35" s="57"/>
       <c r="E35" s="57"/>
       <c r="F35" s="185" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="G35" s="158"/>
       <c r="H35" s="158"/>
@@ -36478,7 +36556,7 @@
     </row>
     <row r="42" spans="2:35">
       <c r="B42" s="97" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="C42" s="92"/>
       <c r="D42" s="92"/>
@@ -36497,7 +36575,7 @@
       <c r="Q42" s="92"/>
       <c r="R42" s="93"/>
       <c r="S42" s="97" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="T42" s="92"/>
       <c r="U42" s="92"/>
@@ -36518,7 +36596,7 @@
     </row>
     <row r="43" spans="2:35">
       <c r="B43" s="94" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="C43" s="95"/>
       <c r="D43" s="95"/>
@@ -36537,7 +36615,7 @@
       <c r="Q43" s="95"/>
       <c r="R43" s="96"/>
       <c r="S43" s="94" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="T43" s="95"/>
       <c r="U43" s="95"/>
@@ -36858,7 +36936,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
       <c r="F52" s="189" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="G52" s="189"/>
       <c r="H52" s="189"/>
@@ -36898,7 +36976,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
       <c r="F53" s="189" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="G53" s="189"/>
       <c r="H53" s="189"/>
@@ -36978,7 +37056,7 @@
       <c r="D55" s="51"/>
       <c r="E55" s="51"/>
       <c r="F55" s="189" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="G55" s="189"/>
       <c r="H55" s="189"/>

</xml_diff>